<commit_message>
runnable test suites commit
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARKO\OneDrive\Desktop\p1\DDT\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96e9be76c92faddd/Desktop/p1/DDT/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4348317D-AB8F-4ACC-9C31-15129C5645E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{4348317D-AB8F-4ACC-9C31-15129C5645E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C9AD532-B5D6-4B6B-B98F-F1465497E533}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{8EFF9ABD-2894-4313-91EB-E956A78B955D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8EFF9ABD-2894-4313-91EB-E956A78B955D}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Suite" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>First Name</t>
   </si>
@@ -105,6 +105,33 @@
   </si>
   <si>
     <t>Account created successfully</t>
+  </si>
+  <si>
+    <t>Run Mode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>Runnable</t>
+  </si>
+  <si>
+    <t>TC001_BankManagerLogin</t>
+  </si>
+  <si>
+    <t>TC002_AddCustomer</t>
+  </si>
+  <si>
+    <t>TC003_OpenAccount</t>
+  </si>
+  <si>
+    <t>TC004_Customers</t>
   </si>
 </sst>
 </file>
@@ -157,6 +184,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,32 +487,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B57C62-BD61-4E20-B7E0-D79E4D2D42C4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77B43D1-5609-4BCD-93FE-2FD35CD783EC}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,8 +573,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -508,8 +590,11 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -522,8 +607,11 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -535,6 +623,9 @@
       </c>
       <c r="D4" t="s">
         <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -544,10 +635,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5E3630-690F-4FAC-A6D2-BCACEE523946}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +647,7 @@
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -566,8 +657,11 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -577,8 +671,11 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -588,8 +685,11 @@
       <c r="C3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -598,6 +698,9 @@
       </c>
       <c r="C4" t="s">
         <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>